<commit_message>
add swin-transformer on decoder
</commit_message>
<xml_diff>
--- a/data/MDMC.xlsx
+++ b/data/MDMC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inkosizhong/lab/MDMC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F68352A-D6BC-764E-8D64-3C32C5BC817F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D3C1E2-0278-0242-A6DA-04FB703C99EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1840" yWindow="500" windowWidth="24640" windowHeight="16040" xr2:uid="{5AF824A9-6FA3-2641-9198-546DAD8D2810}"/>
   </bookViews>
@@ -464,7 +464,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.25280000000000002</c:v>
+                  <c:v>0.25319999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -533,7 +533,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.25409999999999999</c:v>
+                  <c:v>0.2545</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -545,7 +545,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>37.738999999999997</c:v>
+                  <c:v>37.872</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2801,8 +2801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD2DAAB-4498-5143-9909-C8AD4FF4D827}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2924,7 +2924,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="1">
-        <v>0.25280000000000002</v>
+        <v>0.25319999999999998</v>
       </c>
       <c r="G5" s="1">
         <v>37.881</v>
@@ -2950,10 +2950,10 @@
         <v>8</v>
       </c>
       <c r="F6" s="1">
-        <v>0.25409999999999999</v>
+        <v>0.2545</v>
       </c>
       <c r="G6" s="1">
-        <v>37.738999999999997</v>
+        <v>37.872</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -3164,6 +3164,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add FeatureEncoder and FeatureDecoder
</commit_message>
<xml_diff>
--- a/data/MDMC.xlsx
+++ b/data/MDMC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inkosizhong/lab/MDMC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8526A89-1FC3-F443-88A5-24CA65995A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F440C71-390C-5046-8478-4C36099CA6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1840" yWindow="500" windowWidth="24640" windowHeight="16040" xr2:uid="{5AF824A9-6FA3-2641-9198-546DAD8D2810}"/>
   </bookViews>
@@ -640,7 +640,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="3">
-                  <c:v>0.25019999999999998</c:v>
+                  <c:v>0.25059999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -652,7 +652,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="3">
-                  <c:v>38.015999999999998</c:v>
+                  <c:v>38.026000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -665,158 +665,8 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
+          <c:idx val="5"/>
           <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$N$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>37(21)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$N$4:$N$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="3">
-                  <c:v>0.24660000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$O$4:$O$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="3">
-                  <c:v>37.811</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-4414-AA4B-A0E7-D8669BC3B20D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$P$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>38(25)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$P$4:$P$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="3">
-                  <c:v>0.2525</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$Q$4:$Q$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="3">
-                  <c:v>37.729999999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-4414-AA4B-A0E7-D8669BC3B20D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="7"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$R$2</c:f>
@@ -859,7 +709,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="3">
-                  <c:v>0.2329</c:v>
+                  <c:v>0.23400000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -871,7 +721,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="3">
-                  <c:v>37.747999999999998</c:v>
+                  <c:v>37.819000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3300,8 +3150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD2DAAB-4498-5143-9909-C8AD4FF4D827}">
   <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="125" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="143" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3570,10 +3420,10 @@
         <v>37.872</v>
       </c>
       <c r="L7" s="2">
-        <v>0.25019999999999998</v>
+        <v>0.25059999999999999</v>
       </c>
       <c r="M7" s="2">
-        <v>38.015999999999998</v>
+        <v>38.026000000000003</v>
       </c>
       <c r="N7" s="2">
         <v>0.24660000000000001</v>
@@ -3588,10 +3438,10 @@
         <v>37.729999999999997</v>
       </c>
       <c r="R7" s="2">
-        <v>0.2329</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="S7" s="2">
-        <v>37.747999999999998</v>
+        <v>37.819000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:24">

</xml_diff>

<commit_message>
add element level STF_layer
</commit_message>
<xml_diff>
--- a/data/MDMC.xlsx
+++ b/data/MDMC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inkosizhong/lab/MDMC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BEF1BD-8E19-944C-9A93-036CDA072499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CB60C2-8D22-CB45-90ED-2397416971D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1840" yWindow="500" windowWidth="24640" windowHeight="16040" xr2:uid="{5AF824A9-6FA3-2641-9198-546DAD8D2810}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
   <si>
     <t>RGB</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -88,6 +88,14 @@
     <t>MDMC(IR)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>50(21)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>51(21)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -132,7 +140,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -149,6 +157,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -423,6 +434,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.9900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1026</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>0.17460000000000001</c:v>
                 </c:pt>
@@ -438,6 +455,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>33.655000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.042999999999999</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>36.523000000000003</c:v>
                 </c:pt>
@@ -712,7 +735,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="3">
-                  <c:v>0.23400000000000001</c:v>
+                  <c:v>0.2331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -724,7 +747,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="3">
-                  <c:v>37.819000000000003</c:v>
+                  <c:v>37.892000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -733,6 +756,156 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-4414-AA4B-A0E7-D8669BC3B20D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>50(21)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$4:$T$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="3">
+                  <c:v>0.24840000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$U$4:$U$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="3">
+                  <c:v>37.747</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F8C5-B34B-A420-A32B046BF20D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$V$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>51(21)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$V$4:$V$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="3">
+                  <c:v>0.25330000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$W$4:$W$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="3">
+                  <c:v>37.494</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F8C5-B34B-A420-A32B046BF20D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3153,82 +3326,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD2DAAB-4498-5143-9909-C8AD4FF4D827}">
   <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
       <c r="X1" s="4"/>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7">
         <v>19</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6" t="s">
+      <c r="I2" s="7"/>
+      <c r="J2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6" t="s">
+      <c r="K2" s="7"/>
+      <c r="L2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6" t="s">
+      <c r="M2" s="7"/>
+      <c r="N2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6" t="s">
+      <c r="O2" s="7"/>
+      <c r="P2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6" t="s">
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="6"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="W2" s="7"/>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="1" t="s">
@@ -3243,7 +3424,7 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3284,6 +3465,18 @@
         <v>2</v>
       </c>
       <c r="S3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="W3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3303,8 +3496,12 @@
       <c r="E4" s="2">
         <v>256</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="F4" s="2">
+        <v>5.9900000000000002E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>33.655000000000001</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -3334,8 +3531,12 @@
       <c r="E5" s="2">
         <v>512</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="F5" s="2">
+        <v>0.1026</v>
+      </c>
+      <c r="G5" s="2">
+        <v>35.042999999999999</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -3441,10 +3642,22 @@
         <v>37.729999999999997</v>
       </c>
       <c r="R7" s="2">
-        <v>0.23400000000000001</v>
+        <v>0.2331</v>
       </c>
       <c r="S7" s="2">
-        <v>37.819000000000003</v>
+        <v>37.892000000000003</v>
+      </c>
+      <c r="T7" s="6">
+        <v>0.24840000000000001</v>
+      </c>
+      <c r="U7" s="6">
+        <v>37.747</v>
+      </c>
+      <c r="V7" s="6">
+        <v>0.25330000000000003</v>
+      </c>
+      <c r="W7" s="6">
+        <v>37.494</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -3494,25 +3707,25 @@
       <c r="D10" s="1">
         <v>43.545000000000002</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
@@ -3531,19 +3744,19 @@
       <c r="D11" s="1">
         <v>39.484000000000002</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6">
+      <c r="E11" s="7"/>
+      <c r="F11" s="7">
         <v>21</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6">
+      <c r="G11" s="7"/>
+      <c r="H11" s="7">
         <v>28</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6">
+      <c r="I11" s="7"/>
+      <c r="J11" s="7">
         <v>40</v>
       </c>
-      <c r="K11" s="6"/>
+      <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="1">
@@ -3558,7 +3771,7 @@
       <c r="D12" s="1">
         <v>34.988999999999997</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="2" t="s">
         <v>2</v>
       </c>
@@ -3757,7 +3970,10 @@
       <c r="S34" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="19">
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="F1:W1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A1:D1"/>
@@ -3766,7 +3982,6 @@
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="F10:S10"/>
-    <mergeCell ref="F1:S1"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F11:G11"/>

</xml_diff>